<commit_message>
alteracao grafico adicionando temp e alertas
</commit_message>
<xml_diff>
--- a/tempeumidadearduino.xlsx
+++ b/tempeumidadearduino.xlsx
@@ -8,22 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luma\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACC62D1-B42F-43E1-9BDB-CDD789A091FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6680C0B0-4B1C-44FB-AB94-AFA8E3EE218C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfico1" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$52</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$A$52</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$2:$A$52</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$2:$A$52</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$2:$A$52</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$A$2:$A$52</definedName>
-  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -91,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +96,14 @@
       <color rgb="FF000000"/>
       <name val="WordVisi_MSFontService"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -150,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -163,6 +163,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,6 +412,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Umidade</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -442,7 +468,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.4170074798222188E-2"/>
+          <c:y val="0.12156669944280565"/>
+          <c:w val="0.92705645836823591"/>
+          <c:h val="0.80239833590122767"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1548,6 +1584,1202 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Temperatura</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.213648293963254E-2"/>
+          <c:y val="0.12365322516503618"/>
+          <c:w val="0.89972834645669286"/>
+          <c:h val="0.76894742702616714"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TEMPERATURA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>34.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>35.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36.1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>37.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>38.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40.9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40.9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41.1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41.3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>41.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41.7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>39.4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>38.4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>37.4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>36.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>34.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>34.6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>33.4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>32.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>32.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>31.8</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>31.4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>30.6</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>30.2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>29.9</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>30.2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>29.9</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-46A2-43DF-ADCD-67600664FC81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>criticoFrio</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-46A2-43DF-ADCD-67600664FC81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>alertaFrio</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>15.157</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>15.157</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-46A2-43DF-ADCD-67600664FC81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>alertaQuente</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-46A2-43DF-ADCD-67600664FC81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>criticoQuente</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-46A2-43DF-ADCD-67600664FC81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1676266288"/>
+        <c:axId val="1733594576"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1676266288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1733594576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1733594576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1676266288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1628,6 +2860,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2132,6 +3404,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2702,9 +4490,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2724,6 +4512,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC03DC87-27F9-CE87-019F-689B45A2B5E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3031,8 +4855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3117,7 +4941,7 @@
         <v>60</v>
       </c>
       <c r="G2" s="2">
-        <f>(0.33 *A2) + 41.75</f>
+        <f t="shared" ref="G2:G33" si="0">(0.33 *A2) + 41.75</f>
         <v>58.91</v>
       </c>
       <c r="K2" s="3">
@@ -3139,21 +4963,21 @@
         <v>24</v>
       </c>
       <c r="Q2" s="7">
-        <f>(0.77 * K2) - 8.097</f>
+        <f t="shared" ref="Q2:Q33" si="1">(0.77 * K2) - 8.097</f>
         <v>12.308000000000002</v>
       </c>
       <c r="S2" s="1">
         <v>25</v>
       </c>
       <c r="T2" s="2">
-        <f>(0.33 *S2) + 41.75</f>
+        <f t="shared" ref="T2:T33" si="2">(0.33 *S2) + 41.75</f>
         <v>50</v>
       </c>
       <c r="U2" s="5">
         <v>26.1</v>
       </c>
       <c r="V2" s="7">
-        <f>(0.77 * U2) - 8.097</f>
+        <f t="shared" ref="V2:V33" si="3">(0.77 * U2) - 8.097</f>
         <v>12.000000000000002</v>
       </c>
     </row>
@@ -3177,7 +5001,7 @@
         <v>60</v>
       </c>
       <c r="G3" s="2">
-        <f>(0.33 *A3) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>60.230000000000004</v>
       </c>
       <c r="K3" s="4">
@@ -3199,21 +5023,21 @@
         <v>24</v>
       </c>
       <c r="Q3" s="7">
-        <f>(0.77 * K3) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>12.154000000000002</v>
       </c>
       <c r="S3" s="1">
         <v>26</v>
       </c>
       <c r="T3" s="2">
-        <f>(0.33 *S3) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>50.33</v>
       </c>
       <c r="U3" s="3">
         <v>26.2</v>
       </c>
       <c r="V3" s="7">
-        <f>(0.77 * U3) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>12.077</v>
       </c>
     </row>
@@ -3237,7 +5061,7 @@
         <v>60</v>
       </c>
       <c r="G4" s="2">
-        <f>(0.33 *A4) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>60.89</v>
       </c>
       <c r="K4" s="3">
@@ -3259,21 +5083,21 @@
         <v>24</v>
       </c>
       <c r="Q4" s="7">
-        <f>(0.77 * K4) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>12.077</v>
       </c>
       <c r="S4" s="1">
         <v>26</v>
       </c>
       <c r="T4" s="2">
-        <f>(0.33 *S4) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>50.33</v>
       </c>
       <c r="U4" s="3">
         <v>26.2</v>
       </c>
       <c r="V4" s="7">
-        <f>(0.77 * U4) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>12.077</v>
       </c>
     </row>
@@ -3297,7 +5121,7 @@
         <v>60</v>
       </c>
       <c r="G5" s="2">
-        <f>(0.33 *A5) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>59.57</v>
       </c>
       <c r="K5" s="5">
@@ -3319,21 +5143,21 @@
         <v>24</v>
       </c>
       <c r="Q5" s="7">
-        <f>(0.77 * K5) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>12.000000000000002</v>
       </c>
       <c r="S5" s="1">
         <v>27</v>
       </c>
       <c r="T5" s="2">
-        <f>(0.33 *S5) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>50.66</v>
       </c>
       <c r="U5" s="4">
         <v>26.3</v>
       </c>
       <c r="V5" s="7">
-        <f>(0.77 * U5) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>12.154000000000002</v>
       </c>
     </row>
@@ -3357,7 +5181,7 @@
         <v>60</v>
       </c>
       <c r="G6" s="2">
-        <f>(0.33 *A6) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>58.91</v>
       </c>
       <c r="K6" s="3">
@@ -3379,21 +5203,21 @@
         <v>24</v>
       </c>
       <c r="Q6" s="7">
-        <f>(0.77 * K6) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>12.077</v>
       </c>
       <c r="S6" s="1">
         <v>28</v>
       </c>
       <c r="T6" s="2">
-        <f>(0.33 *S6) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>50.99</v>
       </c>
       <c r="U6" s="3">
         <v>26.5</v>
       </c>
       <c r="V6" s="7">
-        <f>(0.77 * U6) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>12.308000000000002</v>
       </c>
     </row>
@@ -3417,7 +5241,7 @@
         <v>60</v>
       </c>
       <c r="G7" s="2">
-        <f>(0.33 *A7) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>58.25</v>
       </c>
       <c r="K7" s="5">
@@ -3439,21 +5263,21 @@
         <v>24</v>
       </c>
       <c r="Q7" s="7">
-        <f>(0.77 * K7) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>13.078000000000001</v>
       </c>
       <c r="S7" s="1">
         <v>29</v>
       </c>
       <c r="T7" s="2">
-        <f>(0.33 *S7) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>51.32</v>
       </c>
       <c r="U7" s="5">
         <v>27.5</v>
       </c>
       <c r="V7" s="7">
-        <f>(0.77 * U7) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>13.078000000000001</v>
       </c>
     </row>
@@ -3477,7 +5301,7 @@
         <v>60</v>
       </c>
       <c r="G8" s="2">
-        <f>(0.33 *A8) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>57.59</v>
       </c>
       <c r="K8" s="5">
@@ -3499,21 +5323,21 @@
         <v>24</v>
       </c>
       <c r="Q8" s="7">
-        <f>(0.77 * K8) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>13.770999999999999</v>
       </c>
       <c r="S8" s="1">
         <v>30</v>
       </c>
       <c r="T8" s="2">
-        <f>(0.33 *S8) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>51.65</v>
       </c>
       <c r="U8" s="3">
         <v>28</v>
       </c>
       <c r="V8" s="7">
-        <f>(0.77 * U8) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>13.463000000000003</v>
       </c>
     </row>
@@ -3537,7 +5361,7 @@
         <v>60</v>
       </c>
       <c r="G9" s="2">
-        <f>(0.33 *A9) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>59.24</v>
       </c>
       <c r="K9" s="3">
@@ -3559,21 +5383,21 @@
         <v>24</v>
       </c>
       <c r="Q9" s="7">
-        <f>(0.77 * K9) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>14.618</v>
       </c>
       <c r="S9" s="1">
         <v>30</v>
       </c>
       <c r="T9" s="2">
-        <f>(0.33 *S9) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>51.65</v>
       </c>
       <c r="U9" s="5">
         <v>28.4</v>
       </c>
       <c r="V9" s="7">
-        <f>(0.77 * U9) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>13.770999999999999</v>
       </c>
     </row>
@@ -3597,7 +5421,7 @@
         <v>60</v>
       </c>
       <c r="G10" s="2">
-        <f>(0.33 *A10) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>56.6</v>
       </c>
       <c r="K10" s="3">
@@ -3619,21 +5443,21 @@
         <v>24</v>
       </c>
       <c r="Q10" s="7">
-        <f>(0.77 * K10) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>15.542</v>
       </c>
       <c r="S10" s="1">
         <v>31</v>
       </c>
       <c r="T10" s="2">
-        <f>(0.33 *S10) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>51.980000000000004</v>
       </c>
       <c r="U10" s="3">
         <v>29.5</v>
       </c>
       <c r="V10" s="7">
-        <f>(0.77 * U10) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>14.618</v>
       </c>
     </row>
@@ -3657,7 +5481,7 @@
         <v>60</v>
       </c>
       <c r="G11" s="2">
-        <f>(0.33 *A11) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>55.94</v>
       </c>
       <c r="K11" s="6">
@@ -3679,21 +5503,21 @@
         <v>24</v>
       </c>
       <c r="Q11" s="7">
-        <f>(0.77 * K11) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>16.466000000000001</v>
       </c>
       <c r="S11" s="1">
         <v>31</v>
       </c>
       <c r="T11" s="2">
-        <f>(0.33 *S11) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>51.980000000000004</v>
       </c>
       <c r="U11" s="3">
         <v>29.9</v>
       </c>
       <c r="V11" s="7">
-        <f>(0.77 * U11) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>14.926</v>
       </c>
     </row>
@@ -3717,7 +5541,7 @@
         <v>60</v>
       </c>
       <c r="G12" s="2">
-        <f>(0.33 *A12) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>55.28</v>
       </c>
       <c r="K12" s="3">
@@ -3739,21 +5563,21 @@
         <v>24</v>
       </c>
       <c r="Q12" s="7">
-        <f>(0.77 * K12) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>17.158999999999999</v>
       </c>
       <c r="S12" s="1">
         <v>32</v>
       </c>
       <c r="T12" s="2">
-        <f>(0.33 *S12) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>52.31</v>
       </c>
       <c r="U12" s="3">
         <v>29.9</v>
       </c>
       <c r="V12" s="7">
-        <f>(0.77 * U12) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>14.926</v>
       </c>
     </row>
@@ -3777,7 +5601,7 @@
         <v>60</v>
       </c>
       <c r="G13" s="2">
-        <f>(0.33 *A13) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>54.29</v>
       </c>
       <c r="K13" s="3">
@@ -3799,21 +5623,21 @@
         <v>24</v>
       </c>
       <c r="Q13" s="7">
-        <f>(0.77 * K13) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>17.852000000000004</v>
       </c>
       <c r="S13" s="1">
         <v>32</v>
       </c>
       <c r="T13" s="2">
-        <f>(0.33 *S13) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>52.31</v>
       </c>
       <c r="U13" s="3">
         <v>30.2</v>
       </c>
       <c r="V13" s="7">
-        <f>(0.77 * U13) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>15.157000000000002</v>
       </c>
     </row>
@@ -3837,7 +5661,7 @@
         <v>60</v>
       </c>
       <c r="G14" s="2">
-        <f>(0.33 *A14) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>53.96</v>
       </c>
       <c r="K14" s="3">
@@ -3859,21 +5683,21 @@
         <v>24</v>
       </c>
       <c r="Q14" s="7">
-        <f>(0.77 * K14) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>18.390999999999998</v>
       </c>
       <c r="S14" s="1">
         <v>33</v>
       </c>
       <c r="T14" s="2">
-        <f>(0.33 *S14) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>52.64</v>
       </c>
       <c r="U14" s="3">
         <v>30.2</v>
       </c>
       <c r="V14" s="7">
-        <f>(0.77 * U14) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>15.157000000000002</v>
       </c>
     </row>
@@ -3897,7 +5721,7 @@
         <v>60</v>
       </c>
       <c r="G15" s="2">
-        <f>(0.33 *A15) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>52.64</v>
       </c>
       <c r="K15" s="3">
@@ -3919,21 +5743,21 @@
         <v>24</v>
       </c>
       <c r="Q15" s="7">
-        <f>(0.77 * K15) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>19.007000000000005</v>
       </c>
       <c r="S15" s="1">
         <v>33</v>
       </c>
       <c r="T15" s="2">
-        <f>(0.33 *S15) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>52.64</v>
       </c>
       <c r="U15" s="3">
         <v>30.6</v>
       </c>
       <c r="V15" s="7">
-        <f>(0.77 * U15) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>15.465000000000002</v>
       </c>
     </row>
@@ -3957,7 +5781,7 @@
         <v>60</v>
       </c>
       <c r="G16" s="2">
-        <f>(0.33 *A16) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>52.31</v>
       </c>
       <c r="K16" s="3">
@@ -3979,21 +5803,21 @@
         <v>24</v>
       </c>
       <c r="Q16" s="7">
-        <f>(0.77 * K16) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>19.700000000000003</v>
       </c>
       <c r="S16" s="1">
         <v>33</v>
       </c>
       <c r="T16" s="2">
-        <f>(0.33 *S16) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>52.64</v>
       </c>
       <c r="U16" s="3">
         <v>30.7</v>
       </c>
       <c r="V16" s="7">
-        <f>(0.77 * U16) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>15.542</v>
       </c>
     </row>
@@ -4017,7 +5841,7 @@
         <v>60</v>
       </c>
       <c r="G17" s="2">
-        <f>(0.33 *A17) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>51.65</v>
       </c>
       <c r="K17" s="3">
@@ -4039,21 +5863,21 @@
         <v>24</v>
       </c>
       <c r="Q17" s="7">
-        <f>(0.77 * K17) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>20.932000000000002</v>
       </c>
       <c r="S17" s="1">
         <v>34</v>
       </c>
       <c r="T17" s="2">
-        <f>(0.33 *S17) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>52.97</v>
       </c>
       <c r="U17" s="3">
         <v>31</v>
       </c>
       <c r="V17" s="7">
-        <f>(0.77 * U17) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>15.773000000000001</v>
       </c>
     </row>
@@ -4077,7 +5901,7 @@
         <v>60</v>
       </c>
       <c r="G18" s="2">
-        <f>(0.33 *A18) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>51.980000000000004</v>
       </c>
       <c r="K18" s="3">
@@ -4099,21 +5923,21 @@
         <v>24</v>
       </c>
       <c r="Q18" s="7">
-        <f>(0.77 * K18) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>21.470999999999997</v>
       </c>
       <c r="S18" s="1">
         <v>35</v>
       </c>
       <c r="T18" s="2">
-        <f>(0.33 *S18) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>53.3</v>
       </c>
       <c r="U18" s="3">
         <v>31.4</v>
       </c>
       <c r="V18" s="7">
-        <f>(0.77 * U18) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>16.081000000000003</v>
       </c>
     </row>
@@ -4137,7 +5961,7 @@
         <v>60</v>
       </c>
       <c r="G19" s="2">
-        <f>(0.33 *A19) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>51.65</v>
       </c>
       <c r="K19" s="3">
@@ -4159,21 +5983,21 @@
         <v>24</v>
       </c>
       <c r="Q19" s="7">
-        <f>(0.77 * K19) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>22.857000000000006</v>
       </c>
       <c r="S19" s="1">
         <v>36</v>
       </c>
       <c r="T19" s="2">
-        <f>(0.33 *S19) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>53.63</v>
       </c>
       <c r="U19" s="3">
         <v>31.8</v>
       </c>
       <c r="V19" s="7">
-        <f>(0.77 * U19) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>16.389000000000003</v>
       </c>
     </row>
@@ -4197,7 +6021,7 @@
         <v>60</v>
       </c>
       <c r="G20" s="2">
-        <f>(0.33 *A20) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>50.99</v>
       </c>
       <c r="K20" s="3">
@@ -4219,21 +6043,21 @@
         <v>24</v>
       </c>
       <c r="Q20" s="7">
-        <f>(0.77 * K20) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>23.011000000000003</v>
       </c>
       <c r="S20" s="1">
         <v>37</v>
       </c>
       <c r="T20" s="2">
-        <f>(0.33 *S20) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>53.96</v>
       </c>
       <c r="U20" s="6">
         <v>31.9</v>
       </c>
       <c r="V20" s="7">
-        <f>(0.77 * U20) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>16.466000000000001</v>
       </c>
     </row>
@@ -4257,7 +6081,7 @@
         <v>60</v>
       </c>
       <c r="G21" s="2">
-        <f>(0.33 *A21) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>50.66</v>
       </c>
       <c r="K21" s="3">
@@ -4279,21 +6103,21 @@
         <v>24</v>
       </c>
       <c r="Q21" s="7">
-        <f>(0.77 * K21) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>23.088000000000001</v>
       </c>
       <c r="S21" s="1">
         <v>37</v>
       </c>
       <c r="T21" s="2">
-        <f>(0.33 *S21) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>53.96</v>
       </c>
       <c r="U21" s="3">
         <v>32.299999999999997</v>
       </c>
       <c r="V21" s="7">
-        <f>(0.77 * U21) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>16.774000000000001</v>
       </c>
     </row>
@@ -4317,7 +6141,7 @@
         <v>60</v>
       </c>
       <c r="G22" s="2">
-        <f>(0.33 *A22) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>50.33</v>
       </c>
       <c r="K22" s="3">
@@ -4339,21 +6163,21 @@
         <v>24</v>
       </c>
       <c r="Q22" s="7">
-        <f>(0.77 * K22) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>23.396000000000001</v>
       </c>
       <c r="S22" s="1">
         <v>38</v>
       </c>
       <c r="T22" s="2">
-        <f>(0.33 *S22) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>54.29</v>
       </c>
       <c r="U22" s="3">
         <v>32.799999999999997</v>
       </c>
       <c r="V22" s="7">
-        <f>(0.77 * U22) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>17.158999999999999</v>
       </c>
     </row>
@@ -4377,7 +6201,7 @@
         <v>60</v>
       </c>
       <c r="G23" s="2">
-        <f>(0.33 *A23) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="K23" s="3">
@@ -4399,21 +6223,21 @@
         <v>24</v>
       </c>
       <c r="Q23" s="7">
-        <f>(0.77 * K23) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>23.242000000000004</v>
       </c>
       <c r="S23" s="1">
         <v>38</v>
       </c>
       <c r="T23" s="2">
-        <f>(0.33 *S23) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>54.29</v>
       </c>
       <c r="U23" s="3">
         <v>32.799999999999997</v>
       </c>
       <c r="V23" s="7">
-        <f>(0.77 * U23) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>17.158999999999999</v>
       </c>
     </row>
@@ -4437,7 +6261,7 @@
         <v>60</v>
       </c>
       <c r="G24" s="2">
-        <f>(0.33 *A24) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>50.33</v>
       </c>
       <c r="K24" s="3">
@@ -4459,21 +6283,21 @@
         <v>24</v>
       </c>
       <c r="Q24" s="7">
-        <f>(0.77 * K24) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>23.396000000000001</v>
       </c>
       <c r="S24" s="1">
         <v>39</v>
       </c>
       <c r="T24" s="2">
-        <f>(0.33 *S24) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>54.620000000000005</v>
       </c>
       <c r="U24" s="3">
         <v>33.4</v>
       </c>
       <c r="V24" s="7">
-        <f>(0.77 * U24) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>17.621000000000002</v>
       </c>
     </row>
@@ -4497,7 +6321,7 @@
         <v>60</v>
       </c>
       <c r="G25" s="2">
-        <f>(0.33 *A25) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>51.32</v>
       </c>
       <c r="K25" s="3">
@@ -4519,21 +6343,21 @@
         <v>24</v>
       </c>
       <c r="Q25" s="7">
-        <f>(0.77 * K25) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>23.472999999999999</v>
       </c>
       <c r="S25" s="1">
         <v>40</v>
       </c>
       <c r="T25" s="2">
-        <f>(0.33 *S25) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>54.95</v>
       </c>
       <c r="U25" s="3">
         <v>33.700000000000003</v>
       </c>
       <c r="V25" s="7">
-        <f>(0.77 * U25) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>17.852000000000004</v>
       </c>
     </row>
@@ -4557,9 +6381,10 @@
         <v>60</v>
       </c>
       <c r="G26" s="2">
-        <f>(0.33 *A26) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>51.980000000000004</v>
       </c>
+      <c r="I26" s="8"/>
       <c r="K26" s="3">
         <v>41.1</v>
       </c>
@@ -4579,21 +6404,21 @@
         <v>24</v>
       </c>
       <c r="Q26" s="7">
-        <f>(0.77 * K26) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>23.550000000000004</v>
       </c>
       <c r="S26" s="1">
         <v>40</v>
       </c>
       <c r="T26" s="2">
-        <f>(0.33 *S26) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>54.95</v>
       </c>
       <c r="U26" s="3">
         <v>34</v>
       </c>
       <c r="V26" s="7">
-        <f>(0.77 * U26) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>18.082999999999998</v>
       </c>
     </row>
@@ -4617,7 +6442,7 @@
         <v>60</v>
       </c>
       <c r="G27" s="2">
-        <f>(0.33 *A27) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>52.31</v>
       </c>
       <c r="K27" s="3">
@@ -4639,21 +6464,21 @@
         <v>24</v>
       </c>
       <c r="Q27" s="7">
-        <f>(0.77 * K27) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>23.704000000000001</v>
       </c>
       <c r="S27" s="1">
         <v>41</v>
       </c>
       <c r="T27" s="2">
-        <f>(0.33 *S27) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>55.28</v>
       </c>
       <c r="U27" s="3">
         <v>34.4</v>
       </c>
       <c r="V27" s="7">
-        <f>(0.77 * U27) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>18.390999999999998</v>
       </c>
     </row>
@@ -4677,7 +6502,7 @@
         <v>60</v>
       </c>
       <c r="G28" s="2">
-        <f>(0.33 *A28) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>52.64</v>
       </c>
       <c r="K28" s="3">
@@ -4699,21 +6524,21 @@
         <v>24</v>
       </c>
       <c r="Q28" s="7">
-        <f>(0.77 * K28) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>23.780999999999999</v>
       </c>
       <c r="S28" s="1">
         <v>42</v>
       </c>
       <c r="T28" s="2">
-        <f>(0.33 *S28) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>55.61</v>
       </c>
       <c r="U28" s="3">
         <v>34.4</v>
       </c>
       <c r="V28" s="7">
-        <f>(0.77 * U28) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>18.390999999999998</v>
       </c>
     </row>
@@ -4737,7 +6562,7 @@
         <v>60</v>
       </c>
       <c r="G29" s="2">
-        <f>(0.33 *A29) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>52.64</v>
       </c>
       <c r="K29" s="3">
@@ -4759,21 +6584,21 @@
         <v>24</v>
       </c>
       <c r="Q29" s="7">
-        <f>(0.77 * K29) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>23.858000000000004</v>
       </c>
       <c r="S29" s="1">
         <v>43</v>
       </c>
       <c r="T29" s="2">
-        <f>(0.33 *S29) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>55.94</v>
       </c>
       <c r="U29" s="3">
         <v>34.6</v>
       </c>
       <c r="V29" s="7">
-        <f>(0.77 * U29) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>18.545000000000002</v>
       </c>
     </row>
@@ -4797,7 +6622,7 @@
         <v>60</v>
       </c>
       <c r="G30" s="2">
-        <f>(0.33 *A30) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>52.97</v>
       </c>
       <c r="K30" s="3">
@@ -4819,21 +6644,21 @@
         <v>24</v>
       </c>
       <c r="Q30" s="7">
-        <f>(0.77 * K30) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>23.935000000000002</v>
       </c>
       <c r="S30" s="1">
         <v>43</v>
       </c>
       <c r="T30" s="2">
-        <f>(0.33 *S30) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>55.94</v>
       </c>
       <c r="U30" s="3">
         <v>35.200000000000003</v>
       </c>
       <c r="V30" s="7">
-        <f>(0.77 * U30) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>19.007000000000005</v>
       </c>
     </row>
@@ -4857,7 +6682,7 @@
         <v>60</v>
       </c>
       <c r="G31" s="2">
-        <f>(0.33 *A31) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>53.3</v>
       </c>
       <c r="K31" s="3">
@@ -4879,21 +6704,21 @@
         <v>24</v>
       </c>
       <c r="Q31" s="7">
-        <f>(0.77 * K31) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>24.012</v>
       </c>
       <c r="S31" s="1">
         <v>45</v>
       </c>
       <c r="T31" s="2">
-        <f>(0.33 *S31) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>56.6</v>
       </c>
       <c r="U31" s="3">
         <v>35.5</v>
       </c>
       <c r="V31" s="7">
-        <f>(0.77 * U31) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>19.238</v>
       </c>
     </row>
@@ -4917,7 +6742,7 @@
         <v>60</v>
       </c>
       <c r="G32" s="2">
-        <f>(0.33 *A32) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>53.63</v>
       </c>
       <c r="K32" s="3">
@@ -4939,21 +6764,21 @@
         <v>24</v>
       </c>
       <c r="Q32" s="7">
-        <f>(0.77 * K32) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>23.858000000000004</v>
       </c>
       <c r="S32" s="1">
         <v>45</v>
       </c>
       <c r="T32" s="2">
-        <f>(0.33 *S32) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>56.6</v>
       </c>
       <c r="U32" s="3">
         <v>36.1</v>
       </c>
       <c r="V32" s="7">
-        <f>(0.77 * U32) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>19.700000000000003</v>
       </c>
     </row>
@@ -4977,7 +6802,7 @@
         <v>60</v>
       </c>
       <c r="G33" s="2">
-        <f>(0.33 *A33) + 41.75</f>
+        <f t="shared" si="0"/>
         <v>53.96</v>
       </c>
       <c r="K33" s="3">
@@ -4999,21 +6824,21 @@
         <v>24</v>
       </c>
       <c r="Q33" s="7">
-        <f>(0.77 * K33) - 8.097</f>
+        <f t="shared" si="1"/>
         <v>22.241</v>
       </c>
       <c r="S33" s="1">
         <v>47</v>
       </c>
       <c r="T33" s="2">
-        <f>(0.33 *S33) + 41.75</f>
+        <f t="shared" si="2"/>
         <v>57.260000000000005</v>
       </c>
       <c r="U33" s="3">
         <v>36.4</v>
       </c>
       <c r="V33" s="7">
-        <f>(0.77 * U33) - 8.097</f>
+        <f t="shared" si="3"/>
         <v>19.930999999999997</v>
       </c>
     </row>
@@ -5037,7 +6862,7 @@
         <v>60</v>
       </c>
       <c r="G34" s="2">
-        <f>(0.33 *A34) + 41.75</f>
+        <f t="shared" ref="G34:G52" si="4">(0.33 *A34) + 41.75</f>
         <v>54.29</v>
       </c>
       <c r="K34" s="3">
@@ -5059,21 +6884,21 @@
         <v>24</v>
       </c>
       <c r="Q34" s="7">
-        <f>(0.77 * K34) - 8.097</f>
+        <f t="shared" ref="Q34:Q52" si="5">(0.77 * K34) - 8.097</f>
         <v>21.470999999999997</v>
       </c>
       <c r="S34" s="1">
         <v>48</v>
       </c>
       <c r="T34" s="2">
-        <f>(0.33 *S34) + 41.75</f>
+        <f t="shared" ref="T34:T65" si="6">(0.33 *S34) + 41.75</f>
         <v>57.59</v>
       </c>
       <c r="U34" s="3">
         <v>37.4</v>
       </c>
       <c r="V34" s="7">
-        <f>(0.77 * U34) - 8.097</f>
+        <f t="shared" ref="V34:V65" si="7">(0.77 * U34) - 8.097</f>
         <v>20.701000000000001</v>
       </c>
     </row>
@@ -5097,7 +6922,7 @@
         <v>60</v>
       </c>
       <c r="G35" s="2">
-        <f>(0.33 *A35) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>54.620000000000005</v>
       </c>
       <c r="K35" s="3">
@@ -5119,21 +6944,21 @@
         <v>24</v>
       </c>
       <c r="Q35" s="7">
-        <f>(0.77 * K35) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>20.701000000000001</v>
       </c>
       <c r="S35" s="1">
         <v>49</v>
       </c>
       <c r="T35" s="2">
-        <f>(0.33 *S35) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>57.92</v>
       </c>
       <c r="U35" s="3">
         <v>37.700000000000003</v>
       </c>
       <c r="V35" s="7">
-        <f>(0.77 * U35) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>20.932000000000002</v>
       </c>
     </row>
@@ -5157,7 +6982,7 @@
         <v>60</v>
       </c>
       <c r="G36" s="2">
-        <f>(0.33 *A36) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>54.95</v>
       </c>
       <c r="K36" s="3">
@@ -5179,21 +7004,21 @@
         <v>24</v>
       </c>
       <c r="Q36" s="7">
-        <f>(0.77 * K36) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>19.930999999999997</v>
       </c>
       <c r="S36" s="1">
         <v>50</v>
       </c>
       <c r="T36" s="2">
-        <f>(0.33 *S36) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>58.25</v>
       </c>
       <c r="U36" s="3">
         <v>38.4</v>
       </c>
       <c r="V36" s="7">
-        <f>(0.77 * U36) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>21.470999999999997</v>
       </c>
     </row>
@@ -5217,7 +7042,7 @@
         <v>60</v>
       </c>
       <c r="G37" s="2">
-        <f>(0.33 *A37) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>54.95</v>
       </c>
       <c r="K37" s="3">
@@ -5239,21 +7064,21 @@
         <v>24</v>
       </c>
       <c r="Q37" s="7">
-        <f>(0.77 * K37) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>19.238</v>
       </c>
       <c r="S37" s="1">
         <v>50</v>
       </c>
       <c r="T37" s="2">
-        <f>(0.33 *S37) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>58.25</v>
       </c>
       <c r="U37" s="3">
         <v>38.4</v>
       </c>
       <c r="V37" s="7">
-        <f>(0.77 * U37) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>21.470999999999997</v>
       </c>
     </row>
@@ -5277,7 +7102,7 @@
         <v>60</v>
       </c>
       <c r="G38" s="2">
-        <f>(0.33 *A38) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>55.61</v>
       </c>
       <c r="K38" s="3">
@@ -5299,21 +7124,21 @@
         <v>24</v>
       </c>
       <c r="Q38" s="7">
-        <f>(0.77 * K38) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>18.390999999999998</v>
       </c>
       <c r="S38" s="1">
         <v>50</v>
       </c>
       <c r="T38" s="2">
-        <f>(0.33 *S38) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>58.25</v>
       </c>
       <c r="U38" s="3">
         <v>39.4</v>
       </c>
       <c r="V38" s="7">
-        <f>(0.77 * U38) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>22.241</v>
       </c>
     </row>
@@ -5337,7 +7162,7 @@
         <v>60</v>
       </c>
       <c r="G39" s="2">
-        <f>(0.33 *A39) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>55.94</v>
       </c>
       <c r="K39" s="3">
@@ -5359,21 +7184,21 @@
         <v>24</v>
       </c>
       <c r="Q39" s="7">
-        <f>(0.77 * K39) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>18.545000000000002</v>
       </c>
       <c r="S39" s="1">
         <v>52</v>
       </c>
       <c r="T39" s="2">
-        <f>(0.33 *S39) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>58.91</v>
       </c>
       <c r="U39" s="3">
         <v>40.200000000000003</v>
       </c>
       <c r="V39" s="7">
-        <f>(0.77 * U39) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>22.857000000000006</v>
       </c>
     </row>
@@ -5397,7 +7222,7 @@
         <v>60</v>
       </c>
       <c r="G40" s="2">
-        <f>(0.33 *A40) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>56.6</v>
       </c>
       <c r="K40" s="3">
@@ -5419,21 +7244,21 @@
         <v>24</v>
       </c>
       <c r="Q40" s="7">
-        <f>(0.77 * K40) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>18.082999999999998</v>
       </c>
       <c r="S40" s="1">
         <v>52</v>
       </c>
       <c r="T40" s="2">
-        <f>(0.33 *S40) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>58.91</v>
       </c>
       <c r="U40" s="3">
         <v>40.4</v>
       </c>
       <c r="V40" s="7">
-        <f>(0.77 * U40) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>23.011000000000003</v>
       </c>
     </row>
@@ -5457,7 +7282,7 @@
         <v>60</v>
       </c>
       <c r="G41" s="2">
-        <f>(0.33 *A41) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>57.260000000000005</v>
       </c>
       <c r="K41" s="3">
@@ -5479,21 +7304,21 @@
         <v>24</v>
       </c>
       <c r="Q41" s="7">
-        <f>(0.77 * K41) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>17.621000000000002</v>
       </c>
       <c r="S41" s="1">
         <v>52</v>
       </c>
       <c r="T41" s="2">
-        <f>(0.33 *S41) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>58.91</v>
       </c>
       <c r="U41" s="3">
         <v>40.5</v>
       </c>
       <c r="V41" s="7">
-        <f>(0.77 * U41) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>23.088000000000001</v>
       </c>
     </row>
@@ -5517,7 +7342,7 @@
         <v>60</v>
       </c>
       <c r="G42" s="2">
-        <f>(0.33 *A42) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>57.92</v>
       </c>
       <c r="K42" s="3">
@@ -5539,21 +7364,21 @@
         <v>24</v>
       </c>
       <c r="Q42" s="7">
-        <f>(0.77 * K42) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>17.158999999999999</v>
       </c>
       <c r="S42" s="1">
         <v>52</v>
       </c>
       <c r="T42" s="2">
-        <f>(0.33 *S42) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>58.91</v>
       </c>
       <c r="U42" s="3">
         <v>40.700000000000003</v>
       </c>
       <c r="V42" s="7">
-        <f>(0.77 * U42) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>23.242000000000004</v>
       </c>
     </row>
@@ -5577,7 +7402,7 @@
         <v>60</v>
       </c>
       <c r="G43" s="2">
-        <f>(0.33 *A43) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>59.57</v>
       </c>
       <c r="K43" s="3">
@@ -5599,21 +7424,21 @@
         <v>24</v>
       </c>
       <c r="Q43" s="7">
-        <f>(0.77 * K43) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>16.774000000000001</v>
       </c>
       <c r="S43" s="1">
         <v>52</v>
       </c>
       <c r="T43" s="2">
-        <f>(0.33 *S43) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>58.91</v>
       </c>
       <c r="U43" s="3">
         <v>40.9</v>
       </c>
       <c r="V43" s="7">
-        <f>(0.77 * U43) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>23.396000000000001</v>
       </c>
     </row>
@@ -5637,7 +7462,7 @@
         <v>60</v>
       </c>
       <c r="G44" s="2">
-        <f>(0.33 *A44) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>58.91</v>
       </c>
       <c r="K44" s="3">
@@ -5659,21 +7484,21 @@
         <v>24</v>
       </c>
       <c r="Q44" s="7">
-        <f>(0.77 * K44) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>16.389000000000003</v>
       </c>
       <c r="S44" s="1">
         <v>53</v>
       </c>
       <c r="T44" s="2">
-        <f>(0.33 *S44) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>59.24</v>
       </c>
       <c r="U44" s="3">
         <v>40.9</v>
       </c>
       <c r="V44" s="7">
-        <f>(0.77 * U44) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>23.396000000000001</v>
       </c>
     </row>
@@ -5697,7 +7522,7 @@
         <v>60</v>
       </c>
       <c r="G45" s="2">
-        <f>(0.33 *A45) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>60.230000000000004</v>
       </c>
       <c r="K45" s="3">
@@ -5719,21 +7544,21 @@
         <v>24</v>
       </c>
       <c r="Q45" s="7">
-        <f>(0.77 * K45) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>16.081000000000003</v>
       </c>
       <c r="S45" s="1">
         <v>54</v>
       </c>
       <c r="T45" s="2">
-        <f>(0.33 *S45) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>59.57</v>
       </c>
       <c r="U45" s="3">
         <v>41</v>
       </c>
       <c r="V45" s="7">
-        <f>(0.77 * U45) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>23.472999999999999</v>
       </c>
     </row>
@@ -5757,7 +7582,7 @@
         <v>60</v>
       </c>
       <c r="G46" s="2">
-        <f>(0.33 *A46) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>58.91</v>
       </c>
       <c r="K46" s="3">
@@ -5779,21 +7604,21 @@
         <v>24</v>
       </c>
       <c r="Q46" s="7">
-        <f>(0.77 * K46) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>15.773000000000001</v>
       </c>
       <c r="S46" s="1">
         <v>54</v>
       </c>
       <c r="T46" s="2">
-        <f>(0.33 *S46) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>59.57</v>
       </c>
       <c r="U46" s="3">
         <v>41.1</v>
       </c>
       <c r="V46" s="7">
-        <f>(0.77 * U46) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>23.550000000000004</v>
       </c>
     </row>
@@ -5817,7 +7642,7 @@
         <v>60</v>
       </c>
       <c r="G47" s="2">
-        <f>(0.33 *A47) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>58.25</v>
       </c>
       <c r="K47" s="3">
@@ -5839,21 +7664,21 @@
         <v>24</v>
       </c>
       <c r="Q47" s="7">
-        <f>(0.77 * K47) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>15.465000000000002</v>
       </c>
       <c r="S47" s="1">
         <v>55</v>
       </c>
       <c r="T47" s="2">
-        <f>(0.33 *S47) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>59.900000000000006</v>
       </c>
       <c r="U47" s="3">
         <v>41.3</v>
       </c>
       <c r="V47" s="7">
-        <f>(0.77 * U47) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>23.704000000000001</v>
       </c>
     </row>
@@ -5877,7 +7702,7 @@
         <v>60</v>
       </c>
       <c r="G48" s="2">
-        <f>(0.33 *A48) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>59.900000000000006</v>
       </c>
       <c r="K48" s="3">
@@ -5899,21 +7724,21 @@
         <v>24</v>
       </c>
       <c r="Q48" s="7">
-        <f>(0.77 * K48) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>15.157000000000002</v>
       </c>
       <c r="S48" s="1">
         <v>55</v>
       </c>
       <c r="T48" s="2">
-        <f>(0.33 *S48) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>59.900000000000006</v>
       </c>
       <c r="U48" s="3">
         <v>41.4</v>
       </c>
       <c r="V48" s="7">
-        <f>(0.77 * U48) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>23.780999999999999</v>
       </c>
     </row>
@@ -5937,7 +7762,7 @@
         <v>60</v>
       </c>
       <c r="G49" s="2">
-        <f>(0.33 *A49) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>58.91</v>
       </c>
       <c r="K49" s="3">
@@ -5959,21 +7784,21 @@
         <v>24</v>
       </c>
       <c r="Q49" s="7">
-        <f>(0.77 * K49) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>14.926</v>
       </c>
       <c r="S49" s="1">
         <v>55</v>
       </c>
       <c r="T49" s="2">
-        <f>(0.33 *S49) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>59.900000000000006</v>
       </c>
       <c r="U49" s="3">
         <v>41.5</v>
       </c>
       <c r="V49" s="7">
-        <f>(0.77 * U49) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>23.858000000000004</v>
       </c>
     </row>
@@ -5997,7 +7822,7 @@
         <v>60</v>
       </c>
       <c r="G50" s="2">
-        <f>(0.33 *A50) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>58.25</v>
       </c>
       <c r="K50" s="3">
@@ -6019,21 +7844,21 @@
         <v>24</v>
       </c>
       <c r="Q50" s="7">
-        <f>(0.77 * K50) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>15.157000000000002</v>
       </c>
       <c r="S50" s="1">
         <v>56</v>
       </c>
       <c r="T50" s="2">
-        <f>(0.33 *S50) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>60.230000000000004</v>
       </c>
       <c r="U50" s="3">
         <v>41.5</v>
       </c>
       <c r="V50" s="7">
-        <f>(0.77 * U50) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>23.858000000000004</v>
       </c>
     </row>
@@ -6057,7 +7882,7 @@
         <v>60</v>
       </c>
       <c r="G51" s="2">
-        <f>(0.33 *A51) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>59.900000000000006</v>
       </c>
       <c r="K51" s="3">
@@ -6079,21 +7904,21 @@
         <v>24</v>
       </c>
       <c r="Q51" s="7">
-        <f>(0.77 * K51) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>14.926</v>
       </c>
       <c r="S51" s="1">
         <v>56</v>
       </c>
       <c r="T51" s="2">
-        <f>(0.33 *S51) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>60.230000000000004</v>
       </c>
       <c r="U51" s="3">
         <v>41.6</v>
       </c>
       <c r="V51" s="7">
-        <f>(0.77 * U51) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>23.935000000000002</v>
       </c>
     </row>
@@ -6117,7 +7942,7 @@
         <v>60</v>
       </c>
       <c r="G52" s="2">
-        <f>(0.33 *A52) + 41.75</f>
+        <f t="shared" si="4"/>
         <v>59.900000000000006</v>
       </c>
       <c r="K52" s="3">
@@ -6139,21 +7964,21 @@
         <v>24</v>
       </c>
       <c r="Q52" s="7">
-        <f>(0.77 * K52) - 8.097</f>
+        <f t="shared" si="5"/>
         <v>13.463000000000003</v>
       </c>
       <c r="S52" s="1">
         <v>58</v>
       </c>
       <c r="T52" s="2">
-        <f>(0.33 *S52) + 41.75</f>
+        <f t="shared" si="6"/>
         <v>60.89</v>
       </c>
       <c r="U52" s="3">
         <v>41.7</v>
       </c>
       <c r="V52" s="7">
-        <f>(0.77 * U52) - 8.097</f>
+        <f t="shared" si="7"/>
         <v>24.012</v>
       </c>
     </row>

</xml_diff>